<commit_message>
Actitime Final Automation Framework
</commit_message>
<xml_diff>
--- a/ActiTime-Automation_Lv4/Controller/data_Controller.xlsx
+++ b/ActiTime-Automation_Lv4/Controller/data_Controller.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\AUTOMATION\WorkSpaceSelenium\ActiTime-Automation\Controller\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9195"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -110,8 +105,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,21 +588,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="15" bestFit="1" customWidth="1"/>
@@ -615,7 +610,7 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -640,10 +635,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -654,10 +649,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -668,10 +663,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -682,10 +677,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -696,10 +691,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -713,7 +708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="45.75" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>

</xml_diff>